<commit_message>
Update on 20250713 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/IPV6直播源汇总/黑龙江移动-IP版.xlsx
+++ b/直播源汇总文档/IPV6直播源汇总/黑龙江移动-IP版.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">地方!$A$1:$H$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">黑龙江!$A$1:$H$265</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$H$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">卫视!$A$1:$H$487</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$H$223</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$H$163</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9600" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9648" uniqueCount="379">
   <si>
     <t>频道</t>
   </si>
@@ -1187,6 +1187,14 @@
   </si>
   <si>
     <t>NEWTV怡伴健康</t>
+  </si>
+  <si>
+    <t>睛彩青少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/3221226508</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -27798,7 +27806,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -28309,7 +28317,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -28324,7 +28332,7 @@
         <v>318</v>
       </c>
       <c r="F20" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G20" t="s">
         <v>119</v>
@@ -28335,7 +28343,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -28350,7 +28358,7 @@
         <v>318</v>
       </c>
       <c r="F21" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G21" t="s">
         <v>119</v>
@@ -28361,7 +28369,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -28376,7 +28384,7 @@
         <v>318</v>
       </c>
       <c r="F22" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G22" t="s">
         <v>119</v>
@@ -28387,7 +28395,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -28402,7 +28410,7 @@
         <v>318</v>
       </c>
       <c r="F23" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G23" t="s">
         <v>119</v>
@@ -28413,7 +28421,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -28428,7 +28436,7 @@
         <v>318</v>
       </c>
       <c r="F24" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G24" t="s">
         <v>119</v>
@@ -28439,7 +28447,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -28454,7 +28462,7 @@
         <v>318</v>
       </c>
       <c r="F25" t="s">
-        <v>289</v>
+        <v>378</v>
       </c>
       <c r="G25" t="s">
         <v>119</v>
@@ -28465,7 +28473,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
@@ -28480,7 +28488,7 @@
         <v>318</v>
       </c>
       <c r="F26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G26" t="s">
         <v>119</v>
@@ -28491,7 +28499,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -28506,7 +28514,7 @@
         <v>318</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G27" t="s">
         <v>119</v>
@@ -28517,7 +28525,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
@@ -28532,7 +28540,7 @@
         <v>318</v>
       </c>
       <c r="F28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G28" t="s">
         <v>119</v>
@@ -28543,7 +28551,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
@@ -28558,7 +28566,7 @@
         <v>318</v>
       </c>
       <c r="F29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G29" t="s">
         <v>119</v>
@@ -28569,7 +28577,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
@@ -28584,7 +28592,7 @@
         <v>318</v>
       </c>
       <c r="F30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G30" t="s">
         <v>119</v>
@@ -28595,7 +28603,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -28610,17 +28618,173 @@
         <v>318</v>
       </c>
       <c r="F31" t="s">
+        <v>289</v>
+      </c>
+      <c r="G31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" t="s">
+        <v>318</v>
+      </c>
+      <c r="F32" t="s">
         <v>290</v>
       </c>
-      <c r="G31" t="s">
-        <v>119</v>
-      </c>
-      <c r="H31" s="1" t="s">
+      <c r="G32" t="s">
+        <v>119</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E33" t="s">
+        <v>318</v>
+      </c>
+      <c r="F33" t="s">
+        <v>290</v>
+      </c>
+      <c r="G33" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" t="s">
+        <v>318</v>
+      </c>
+      <c r="F34" t="s">
+        <v>290</v>
+      </c>
+      <c r="G34" t="s">
+        <v>119</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E35" t="s">
+        <v>318</v>
+      </c>
+      <c r="F35" t="s">
+        <v>290</v>
+      </c>
+      <c r="G35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E36" t="s">
+        <v>318</v>
+      </c>
+      <c r="F36" t="s">
+        <v>290</v>
+      </c>
+      <c r="G36" t="s">
+        <v>119</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E37" t="s">
+        <v>318</v>
+      </c>
+      <c r="F37" t="s">
+        <v>290</v>
+      </c>
+      <c r="G37" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H31"/>
+  <autoFilter ref="A1:H37"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20250713 part 9
</commit_message>
<xml_diff>
--- a/直播源汇总文档/IPV6直播源汇总/黑龙江移动-IP版.xlsx
+++ b/直播源汇总文档/IPV6直播源汇总/黑龙江移动-IP版.xlsx
@@ -13,6 +13,7 @@
     <sheet name="地方" sheetId="4" r:id="rId4"/>
     <sheet name="体育" sheetId="5" r:id="rId5"/>
     <sheet name="娱乐" sheetId="6" r:id="rId6"/>
+    <sheet name="所有频道URL" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">地方!$A$1:$H$31</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9648" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9848" uniqueCount="578">
   <si>
     <t>频道</t>
   </si>
@@ -1195,6 +1196,603 @@
   <si>
     <t>/3221226508</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226016/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226514/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226559/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225588/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226021/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226428/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226007/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226019/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225603/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226010/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225733/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226008/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225734/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225730/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226473/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226565/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225597/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225731/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226568/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226011/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226537/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226571/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225732/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226591/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226476/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225601/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226100/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225765/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225604/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226517/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226543/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226520/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226431/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225602/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225652/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226425/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225783/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225659/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226391/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226498/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225728/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226450/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226251/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226439/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225618/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226409/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226463/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225735/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226345/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226336/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225620/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226341/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226377/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225633/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226522/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226248/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226374/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226549/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226380/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226474/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225626/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226383/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226465/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225639/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226445/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226406/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225623/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226448/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226480/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226320/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225627/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226477/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226501/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225610/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226307/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226430/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226397/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226386/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225613/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226310/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226495/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226344/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226504/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225660/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225619/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226546/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226254/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225634/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226389/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225632/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226454/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225628/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226323/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225655/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226456/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226507/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225624/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226392/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225625/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226457/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225739/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226313/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226510/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226338/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226513/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225740/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226459/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226395/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225638/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226433/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225635/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226460/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226516/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226444/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225612/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226339/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226342/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226327/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226585/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226582/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226532/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226531/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226525/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226467/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226419/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226421/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226298/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226365/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226239/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226424/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226301/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226427/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226330/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226368/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226242/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226492/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226304/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226371/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226434/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226558/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225760/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226552/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225762/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226526/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226437/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226413/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226555/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226493/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226534/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226496/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226484/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226523/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226499/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226529/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226502/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226451/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226416/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226535/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226422/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226410/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226481/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225657/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225729/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225654/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225656/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225653/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226124/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226147/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226469/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226508/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226472/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226398/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225669/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225716/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225717/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225715/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225714/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225685/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225675/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225741/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225663/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225671/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225743/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225662/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225742/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225677/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225666/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225665/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225670/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225672/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221226505/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225674/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225676/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225668/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225664/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225683/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225680/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225719/index.m3u8</t>
+  </si>
+  <si>
+    <t>/ottrrs.hl.chinamobile.com/PLTV/88888888/224/3221225673/index.m3u8</t>
   </si>
 </sst>
 </file>
@@ -33051,4 +33649,1022 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A200"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="73.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A57" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A81" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A82" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A83" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A101" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A103" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A105" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A106" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A107" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A108" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A109" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A110" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A111" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A112" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A113" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A115" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A116" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A117" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A119" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A120" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A121" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A122" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A124" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A125" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A126" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A127" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A129" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A131" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A133" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A134" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A136" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A137" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A139" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A146" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A149" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A154" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A156" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A162" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A163" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A165" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A166" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A167" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A168" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A169" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A170" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A171" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A172" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A173" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A174" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A175" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A176" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A177" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A178" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A179" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A180" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A181" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A182" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A183" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A184" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A185" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A186" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A187" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A188" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A189" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A190" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A191" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A192" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A193" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A194" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A195" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A196" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A197" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A198" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A199" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A200" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>